<commit_message>
Update data to 2021.2
</commit_message>
<xml_diff>
--- a/data/desc.xlsx
+++ b/data/desc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migareev\Documents\macro_forecast_russia\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migareev\Documents\macro_nowcast_russia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="108">
   <si>
     <t>Показатель</t>
   </si>
@@ -351,6 +351,12 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>export_and_stocks</t>
+  </si>
+  <si>
+    <t>Экспорт и инвестиции в запасы в постоянных ценах</t>
   </si>
 </sst>
 </file>
@@ -704,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1938,6 +1944,32 @@
         <v>104</v>
       </c>
     </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48">
+        <v>27</v>
+      </c>
+      <c r="D48" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:H1048576">
     <sortCondition ref="C1"/>

</xml_diff>